<commit_message>
add interface case 4
</commit_message>
<xml_diff>
--- a/casedata/WCSQueryInterface.xlsx
+++ b/casedata/WCSQueryInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24285" windowHeight="12465"/>
+    <workbookView windowWidth="19545" windowHeight="10365"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>apiCaseName</t>
   </si>
@@ -108,6 +108,36 @@
  "warehouseArea": "11111111111111111111",
  "bucketCode": "1003"
 }</t>
+  </si>
+  <si>
+    <t>case10</t>
+  </si>
+  <si>
+    <t>http://192.168.21.188:8080/wcs/agv/status?warehouseId=60001111&amp;agvCode=agv001</t>
+  </si>
+  <si>
+    <t>Get</t>
+  </si>
+  <si>
+    <t>{"agvCode":null,"warehouseId":null,"onlineState":null,"wcsJobId":null,"jobStatus":null,"msg":"could not find any info of agv001"}</t>
+  </si>
+  <si>
+    <t>case11</t>
+  </si>
+  <si>
+    <t>case12</t>
+  </si>
+  <si>
+    <t>http://192.168.21.188:8080/wcs/agv/status?warehouseId=6000111111&amp;agvCode=JX-PSS-AGV-192168001001</t>
+  </si>
+  <si>
+    <t>case13</t>
+  </si>
+  <si>
+    <t>http://192.168.21.188:8080/wcs/agv/status?warehouseId=60001&amp;agvCode=JX-PSS-AGV-192168001001</t>
+  </si>
+  <si>
+    <t>{"agvCode":"JX-PSS-AGV-192168001001","warehouseId":60001,"onlineState":"ONLINE","wcsJobId":4234,"jobStatus":"MOVE_COMPLETED","msg":"success"}</t>
   </si>
 </sst>
 </file>
@@ -115,12 +145,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,18 +175,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <u/>
+      <sz val="10.5"/>
+      <color rgb="FF800080"/>
+      <name val="Chinese Quote"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -168,31 +191,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -205,14 +206,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,7 +222,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,22 +244,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,17 +274,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,187 +319,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,17 +513,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,9 +569,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -519,7 +582,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,47 +610,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -581,10 +618,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -593,137 +630,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -735,6 +772,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1084,16 +1124,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="2" max="2" width="89.5583333333333" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="13.625" customWidth="1"/>
     <col min="5" max="5" width="14.75" customWidth="1"/>
@@ -1234,12 +1274,77 @@
         <v>23</v>
       </c>
     </row>
+    <row r="7" ht="40.5" spans="1:8">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="40.5" spans="1:8">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="http://192.168.21.188:8080/wcs/bucket/query" tooltip="http://192.168.21.188:8080/wcs/bucket/query"/>
     <hyperlink ref="B4" r:id="rId1" display="http://192.168.21.188:8080/wcs/bucket/query" tooltip="http://192.168.21.188:8080/wcs/bucket/query"/>
     <hyperlink ref="B5" r:id="rId1" display="http://192.168.21.188:8080/wcs/bucket/query" tooltip="http://192.168.21.188:8080/wcs/bucket/query"/>
     <hyperlink ref="B6" r:id="rId1" display="http://192.168.21.188:8080/wcs/bucket/query" tooltip="http://192.168.21.188:8080/wcs/bucket/query"/>
+    <hyperlink ref="B7" r:id="rId2" display="http://192.168.21.188:8080/wcs/agv/status?warehouseId=60001111&amp;agvCode=agv001" tooltip="http://192.168.21.188:8080/wcs/agv/status?warehouseId=60001111&amp;agvCode=agv001"/>
+    <hyperlink ref="B9" r:id="rId3" display="http://192.168.21.188:8080/wcs/agv/status?warehouseId=6000111111&amp;agvCode=JX-PSS-AGV-192168001001"/>
+    <hyperlink ref="B8" r:id="rId2" display="http://192.168.21.188:8080/wcs/agv/status?warehouseId=60001111&amp;agvCode=agv001"/>
   </hyperlinks>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
add sql and param
</commit_message>
<xml_diff>
--- a/casedata/WCSQueryInterface.xlsx
+++ b/casedata/WCSQueryInterface.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19545" windowHeight="10365"/>
+    <workbookView windowWidth="19545" windowHeight="9765"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37">
   <si>
     <t>apiCaseName</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Expectation</t>
+  </si>
+  <si>
+    <t>strategyType</t>
+  </si>
+  <si>
+    <t>optionType</t>
+  </si>
+  <si>
+    <t>optionInfo</t>
   </si>
   <si>
     <t>case1</t>
@@ -145,10 +154,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -183,6 +192,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -191,7 +215,73 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,16 +295,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,89 +313,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,187 +328,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,45 +519,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -563,26 +533,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,8 +555,67 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,10 +627,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -630,16 +639,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -651,112 +660,112 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1124,13 +1133,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="13.25" customWidth="1"/>
     <col min="2" max="2" width="89.5583333333333" customWidth="1"/>
@@ -1142,7 +1151,7 @@
     <col min="8" max="8" width="64.85" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1166,174 +1175,183 @@
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" ht="148.5" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="148.5" spans="1:6">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" ht="148.5" spans="1:8">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" ht="148.5" spans="1:6">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" ht="175.5" spans="1:6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" ht="40.5" spans="1:8">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" ht="40.5" spans="1:8">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>